<commit_message>
Add final site orientation
</commit_message>
<xml_diff>
--- a/primerdata_allspecies.xlsx
+++ b/primerdata_allspecies.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10645" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10650" uniqueCount="286">
   <si>
     <t>No.</t>
   </si>
@@ -6481,8 +6481,8 @@
       <c r="DR15" t="s">
         <v>281</v>
       </c>
-      <c r="DS15" t="e">
-        <v>#N/A</v>
+      <c r="DS15" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="16">
@@ -13159,8 +13159,8 @@
       <c r="DR33" t="s">
         <v>281</v>
       </c>
-      <c r="DS33" t="e">
-        <v>#N/A</v>
+      <c r="DS33" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="34">
@@ -19466,8 +19466,8 @@
       <c r="DR50" t="s">
         <v>281</v>
       </c>
-      <c r="DS50" t="e">
-        <v>#N/A</v>
+      <c r="DS50" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="51">
@@ -26144,8 +26144,8 @@
       <c r="DR68" t="s">
         <v>281</v>
       </c>
-      <c r="DS68" t="e">
-        <v>#N/A</v>
+      <c r="DS68" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="69">
@@ -32451,8 +32451,8 @@
       <c r="DR85" t="s">
         <v>281</v>
       </c>
-      <c r="DS85" t="e">
-        <v>#N/A</v>
+      <c r="DS85" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="86">

</xml_diff>